<commit_message>
rename "Government" to "Public Administration". This was the official term used.
</commit_message>
<xml_diff>
--- a/formats/sectors.xlsx
+++ b/formats/sectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Desktop/git/enisa/NIS-sectors/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A7BB3C1-5B84-5D44-9592-014F5CB3229C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0629697-DA77-2743-B539-EAC9F2470047}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1460" windowWidth="24640" windowHeight="14000" xr2:uid="{548CAF4F-702E-CE42-BB4F-8E3ED54A21EE}"/>
   </bookViews>
@@ -155,9 +155,6 @@
     <t>DNS-Name-Registries</t>
   </si>
   <si>
-    <t>Government</t>
-  </si>
-  <si>
     <t>Öffentliche Verwaltung</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Unbekannt</t>
+  </si>
+  <si>
+    <t>Public Administration</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7F4774-0561-0F48-ABFC-C56502F1256F}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -827,16 +829,16 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
       <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
         <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -847,16 +849,16 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
       </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
         <v>38</v>
-      </c>
-      <c r="F16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -867,16 +869,16 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
       <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
         <v>40</v>
-      </c>
-      <c r="F17" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>